<commit_message>
Formater and Action Level further along, needs refinement
</commit_message>
<xml_diff>
--- a/Side by side 10.10.2016.xlsx
+++ b/Side by side 10.10.2016.xlsx
@@ -3430,7 +3430,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -3443,16 +3443,19 @@
   </sheetPr>
   <dimension ref="A1:O189"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="Q4" sqref="Q4"/>
+    <sheetView tabSelected="1" topLeftCell="A171" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8:E189"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="35" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.75" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="11" width="10.625" style="1" customWidth="1"/>
-    <col min="12" max="13" width="10.75" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="5" width="10.625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="19.75" style="1" customWidth="1"/>
+    <col min="7" max="11" width="10.625" style="1" customWidth="1"/>
+    <col min="12" max="12" width="10.75" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="23.625" style="1" customWidth="1"/>
     <col min="14" max="14" width="12.75" style="1" customWidth="1"/>
     <col min="15" max="15" width="13" style="1" customWidth="1"/>
     <col min="16" max="16384" width="9" style="1"/>
@@ -12920,21 +12923,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100A57ED4EB561C6E47B95AFA1F7078C92B" ma:contentTypeVersion="0" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="fbfa1ddbedfa3054f20c5104949b8bd5">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="1b05d82d297216baf5b26c55225140df">
     <xsd:element name="properties">
@@ -13048,10 +13036,33 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C569D7FD-C17E-4554-953E-032691D77DCF}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7773A8F4-1F6E-46B9-83F6-CF8F5EA27EC8}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -13072,17 +13083,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7773A8F4-1F6E-46B9-83F6-CF8F5EA27EC8}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C569D7FD-C17E-4554-953E-032691D77DCF}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>